<commit_message>
va_stoch - refining scenarios
</commit_message>
<xml_diff>
--- a/projects/va_stoch/data/scenarios.xlsx
+++ b/projects/va_stoch/data/scenarios.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF05370D-E8BB-458C-A49C-A10E5D49DFEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F2F6AB-2DAF-403D-AC4E-041B5FC2A6B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="85">
   <si>
     <t>Scenario</t>
   </si>
@@ -476,6 +476,9 @@
   </si>
   <si>
     <t>B2050</t>
+  </si>
+  <si>
+    <t>B2030</t>
   </si>
 </sst>
 </file>
@@ -575,7 +578,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1038,30 +1069,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8" customWidth="1"/>
+    <col min="2" max="4" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1071,8 +1105,11 @@
       <c r="C2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1082,8 +1119,11 @@
       <c r="C3" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1093,8 +1133,11 @@
       <c r="C4" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1104,8 +1147,11 @@
       <c r="C5">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1115,8 +1161,11 @@
       <c r="C6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -1126,8 +1175,11 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>75</v>
       </c>
@@ -1137,8 +1189,11 @@
       <c r="C8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>27</v>
       </c>
@@ -1148,8 +1203,11 @@
       <c r="C9" s="14" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>29</v>
       </c>
@@ -1159,8 +1217,11 @@
       <c r="C10" s="14">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>30</v>
       </c>
@@ -1170,9 +1231,17 @@
       <c r="C11" s="14">
         <v>1000</v>
       </c>
+      <c r="D11" s="14">
+        <v>1000</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:XFD1048576">
+  <conditionalFormatting sqref="B2:B1048576 D2:XFD1048576">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C1048576">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -1184,10 +1253,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1195,18 +1264,21 @@
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1216,8 +1288,11 @@
       <c r="C2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>78</v>
       </c>
@@ -1227,8 +1302,11 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1238,8 +1316,11 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1249,8 +1330,11 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>80</v>
       </c>
@@ -1260,8 +1344,11 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1271,8 +1358,11 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -1282,8 +1372,11 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1293,8 +1386,11 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>79</v>
       </c>
@@ -1304,8 +1400,11 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -1315,8 +1414,11 @@
       <c r="C11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1326,8 +1428,11 @@
       <c r="C12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -1337,8 +1442,11 @@
       <c r="C13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1348,8 +1456,11 @@
       <c r="C14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -1359,8 +1470,11 @@
       <c r="C15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
@@ -1370,8 +1484,11 @@
       <c r="C16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -1381,8 +1498,11 @@
       <c r="C17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1392,8 +1512,11 @@
       <c r="C18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -1403,8 +1526,11 @@
       <c r="C19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -1414,8 +1540,11 @@
       <c r="C20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -1425,8 +1554,11 @@
       <c r="C21" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -1436,8 +1568,11 @@
       <c r="C22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
@@ -1447,9 +1582,17 @@
       <c r="C23" t="s">
         <v>17</v>
       </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:XFD1048576">
+  <conditionalFormatting sqref="B24:XFD1048576 B2:B23 D2:XFD23">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C23">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -1461,10 +1604,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1472,18 +1615,21 @@
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1493,8 +1639,11 @@
       <c r="C2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1504,8 +1653,11 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1515,8 +1667,11 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1526,8 +1681,11 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1537,8 +1695,11 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1548,8 +1709,11 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -1559,8 +1723,11 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -1570,9 +1737,17 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:XFD1048576">
+  <conditionalFormatting sqref="B10:XFD1048576 B2:B9 D2:XFD9">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C9">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -1583,10 +1758,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1594,18 +1769,21 @@
     <col min="1" max="1" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -1615,8 +1793,11 @@
       <c r="C2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -1626,8 +1807,11 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1637,8 +1821,11 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1648,8 +1835,11 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1659,18 +1849,21 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -1680,8 +1873,11 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -1691,8 +1887,11 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -1702,23 +1901,26 @@
       <c r="C11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -1728,9 +1930,17 @@
       <c r="C15" t="s">
         <v>17</v>
       </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:XFD1048576">
+  <conditionalFormatting sqref="B16:XFD1048576 B2:B15 D2:XFD15">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C15">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
va_stoch - refining scenarios and pre-processing
</commit_message>
<xml_diff>
--- a/projects/va_stoch/data/scenarios.xlsx
+++ b/projects/va_stoch/data/scenarios.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F2F6AB-2DAF-403D-AC4E-041B5FC2A6B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB57729E-B68B-4CCC-A220-4EFC0707CC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="91">
   <si>
     <t>Scenario</t>
   </si>
@@ -472,13 +472,31 @@
     <t>OFFSHORE_TRANS</t>
   </si>
   <si>
-    <t>B2035</t>
-  </si>
-  <si>
-    <t>B2050</t>
-  </si>
-  <si>
-    <t>B2030</t>
+    <t>E_PV_DIST_RES</t>
+  </si>
+  <si>
+    <t>E_SCO2</t>
+  </si>
+  <si>
+    <t>E_OCAES</t>
+  </si>
+  <si>
+    <t>E_BECCS</t>
+  </si>
+  <si>
+    <t>NATGAS_TO_CCS</t>
+  </si>
+  <si>
+    <t>BIO_TO_CCS</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -502,7 +520,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -539,6 +557,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -552,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -574,6 +598,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1071,8 +1096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1086,13 +1111,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1242,7 +1267,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1253,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1269,13 +1294,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1586,14 +1611,58 @@
         <v>17</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B24:XFD1048576 B2:B23 D2:XFD23">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C23">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1607,7 +1676,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1620,13 +1689,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1743,12 +1812,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10:XFD1048576 B2:B9 D2:XFD9">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C9">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1758,10 +1827,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1774,13 +1843,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1934,9 +2003,28 @@
         <v>17</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B16:XFD1048576 B2:B15 D2:XFD15">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>